<commit_message>
deverlop Internal moving Wagon
</commit_message>
<xml_diff>
--- a/Documents/Таблицы ИДС/Таблицы внутреннего перемещения.xlsx
+++ b/Documents/Таблицы ИДС/Таблицы внутреннего перемещения.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Visual Studio 2013\Projects\Work\IDS RailWay\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Мои документы\Visual Studio 2013\Projects\Work\IDS RailWay\Documents\Таблицы ИДС\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719A2413-1A10-4882-99C3-5D9CA3E72BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E51CBB86-B8F8-472E-9C89-3F4D9548AFD3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$H$49</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -386,9 +385,6 @@
     <t>WagonInternalRoutes</t>
   </si>
   <si>
-    <t>WagonDislocation</t>
-  </si>
-  <si>
     <t>Directory_Wagons</t>
   </si>
   <si>
@@ -444,34 +440,6 @@
   </si>
   <si>
     <t>[Directory_TypeWagons]</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">num -&gt; [WagonInternalRoutes] -&gt; id -&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">последняя запись </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[WagonDislocation]</t>
-    </r>
   </si>
   <si>
     <r>
@@ -908,12 +876,18 @@
   <si>
     <t>бит</t>
   </si>
+  <si>
+    <t>WagonInternalMovement</t>
+  </si>
+  <si>
+    <t>num -&gt; [WagonInternalRoutes] -&gt; id -&gt; последняя запись [WagonInternalMovement]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -976,13 +950,26 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -994,10 +981,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1011,9 +999,14 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1053,7 +1046,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1383,11 +1376,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9E2C63-89BB-4F8E-B771-C1511B4E1CE3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1405,19 +1398,19 @@
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1433,10 +1426,10 @@
         <v>113</v>
       </c>
       <c r="D2" t="s">
-        <v>116</v>
+        <v>183</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>136</v>
+        <v>184</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>1</v>
@@ -1456,7 +1449,7 @@
         <v>115</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>2</v>
@@ -1475,17 +1468,17 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>125</v>
+      <c r="E5" s="8" t="s">
+        <v>124</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1497,13 +1490,13 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" t="s">
         <v>128</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>6</v>
@@ -1523,13 +1516,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>10</v>
@@ -1549,13 +1542,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" t="s">
         <v>134</v>
       </c>
-      <c r="D8" t="s">
-        <v>135</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
@@ -1575,13 +1568,13 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>15</v>
@@ -1601,13 +1594,13 @@
         <v>16</v>
       </c>
       <c r="C10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>17</v>
@@ -1627,13 +1620,13 @@
         <v>18</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>19</v>
@@ -1653,13 +1646,13 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>22</v>
@@ -1679,7 +1672,7 @@
         <v>23</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
@@ -1700,13 +1693,13 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>26</v>
@@ -1726,13 +1719,13 @@
         <v>27</v>
       </c>
       <c r="C15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>27</v>
@@ -1752,13 +1745,13 @@
         <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D16" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>29</v>
@@ -1778,13 +1771,13 @@
         <v>30</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>31</v>
@@ -1804,13 +1797,13 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>34</v>
@@ -1830,16 +1823,16 @@
         <v>35</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H19" t="s">
         <v>32</v>
@@ -1850,13 +1843,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
@@ -1877,13 +1870,13 @@
         <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>39</v>
@@ -1900,16 +1893,16 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>41</v>
@@ -1923,10 +1916,10 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>42</v>
@@ -1943,7 +1936,7 @@
         <v>43</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>44</v>
@@ -1963,7 +1956,7 @@
         <v>46</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>47</v>
@@ -1983,10 +1976,10 @@
         <v>49</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1997,7 +1990,7 @@
         <v>50</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>51</v>
@@ -2017,7 +2010,7 @@
         <v>53</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>54</v>
@@ -2037,7 +2030,7 @@
         <v>56</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>57</v>
@@ -2054,7 +2047,7 @@
         <v>59</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>60</v>
@@ -2071,7 +2064,7 @@
         <v>61</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>62</v>
@@ -2088,10 +2081,10 @@
         <v>63</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>64</v>
@@ -2108,10 +2101,10 @@
         <v>65</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>66</v>
@@ -2131,7 +2124,7 @@
         <v>68</v>
       </c>
       <c r="D34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
@@ -2152,7 +2145,7 @@
         <v>70</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2" t="s">
@@ -2173,7 +2166,7 @@
         <v>73</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E36" s="2"/>
       <c r="F36" s="2" t="s">
@@ -2194,7 +2187,7 @@
         <v>75</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2" t="s">
@@ -2413,7 +2406,7 @@
         <v>100</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E49" s="2"/>
       <c r="F49" s="2" t="s">
@@ -2518,7 +2511,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{F9F2818B-13C5-4AF4-A4DD-578835C011BE}"/>
+  <autoFilter ref="A1:H49"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
deverlop WSD view Wagons
</commit_message>
<xml_diff>
--- a/Documents/Таблицы ИДС/Таблицы внутреннего перемещения.xlsx
+++ b/Documents/Таблицы ИДС/Таблицы внутреннего перемещения.xlsx
@@ -1046,7 +1046,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000008040000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1379,8 +1379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>